<commit_message>
Fill some missing data of higher education
</commit_message>
<xml_diff>
--- a/数据收集-高等教育/05-补全计划/创建时间补全v20221227_WH_20230105.xlsx
+++ b/数据收集-高等教育/05-补全计划/创建时间补全v20221227_WH_20230105.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25200" windowHeight="12090"/>
+    <workbookView windowWidth="28800" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="创建时间补全v20221227_WH_空表" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="151">
   <si>
     <t>学校名称</t>
   </si>
@@ -34,6 +34,9 @@
     <t>沈阳工业大学工程学院</t>
   </si>
   <si>
+    <t>2004年1月</t>
+  </si>
+  <si>
     <t>LJJ_20221213</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>公安部管理干部学院</t>
   </si>
   <si>
+    <t>1978年6月</t>
+  </si>
+  <si>
     <t>https://m.maigoo.com/citiao/2656.html</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t>天津市渤海化工职工学院</t>
   </si>
   <si>
+    <t>1987年2月19日</t>
+  </si>
+  <si>
     <t>http://tianjin0160194.11467.com/about.asp</t>
   </si>
   <si>
@@ -136,18 +145,21 @@
     <t>https://www.maigoo.com/citiao/2703.html</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>吉林市职工大学</t>
   </si>
   <si>
+    <t>1999年2月3日</t>
+  </si>
+  <si>
     <t>http://www.11467.com/jilinshi/co/9379.htm</t>
   </si>
   <si>
     <t>吉林开放大学</t>
   </si>
   <si>
+    <t>1979年2月</t>
+  </si>
+  <si>
     <t>https://www.maigoo.com/citiao/2724.html</t>
   </si>
   <si>
@@ -184,6 +196,9 @@
     <t>鹤岗矿务局职工大学</t>
   </si>
   <si>
+    <t>1958年1月</t>
+  </si>
+  <si>
     <t>https://baike.baidu.com/item/%E9%B9%A4%E5%B2%97%E7%9F%BF%E5%8A%A1%E5%B1%80%E8%81%8C%E5%B7%A5%E5%A4%A7%E5%AD%A6/164519?fr=aladdin</t>
   </si>
   <si>
@@ -221,6 +236,9 @@
   </si>
   <si>
     <t>温州市工人业余大学</t>
+  </si>
+  <si>
+    <t>1979年8月</t>
   </si>
   <si>
     <t>https://xq.wztvu.com/Col/Col60/Index.aspx</t>
@@ -357,6 +375,9 @@
     <t>株洲市职工大学</t>
   </si>
   <si>
+    <t>1980年10月</t>
+  </si>
+  <si>
     <t>https://www.diyifanwen.com/college/hunangaoxiao/0711402241994014348.htm</t>
   </si>
   <si>
@@ -366,6 +387,9 @@
     <t>广东省职工体育运动技术学院/广东体育职业技术学院？</t>
   </si>
   <si>
+    <t>1956年8月</t>
+  </si>
+  <si>
     <t>https://zhidao.baidu.com/question/1700088312054264068.html</t>
   </si>
   <si>
@@ -375,6 +399,9 @@
     <t>成都冶金职工大学</t>
   </si>
   <si>
+    <t>1975年6月</t>
+  </si>
+  <si>
     <t>https://www.maigoo.com/citiao/2876.html</t>
   </si>
   <si>
@@ -445,6 +472,9 @@
   </si>
   <si>
     <t>新疆生产建设兵团教育学院</t>
+  </si>
+  <si>
+    <t>1983年1月1日</t>
   </si>
   <si>
     <t>http://www.11467.com/shihezi/co/2049.htm</t>
@@ -492,30 +522,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -527,19 +559,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -558,14 +581,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -575,10 +590,24 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -592,7 +621,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -600,22 +637,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,8 +650,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -650,12 +680,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -668,169 +848,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,17 +874,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -874,20 +916,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -907,30 +946,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -941,232 +956,244 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="57" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="57" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1447,18 +1474,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3666666666667" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="10.3653846153846" defaultRowHeight="17.6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="34.5416666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6333333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1833333333333" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.3666666666667" style="1"/>
+    <col min="1" max="1" width="34.5384615384615" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7692307692308" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1826923076923" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.3653846153846" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1482,682 +1509,679 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
-        <v>37987</v>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2">
-        <v>28642</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="4">
-        <v>31827</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="4">
-        <v>36194</v>
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2">
-        <v>28887</v>
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="2">
-        <v>21186</v>
+        <v>59</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="5">
-        <v>29068</v>
+        <v>73</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B36" s="2">
-        <v>29495</v>
+        <v>115</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="2">
-        <v>20668</v>
+      <c r="A37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="2">
-        <v>27546</v>
+        <v>123</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B45" s="4">
-        <v>30317</v>
+        <v>148</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>